<commit_message>
wrote an updated circular prompt after 1st testing of phase 1
</commit_message>
<xml_diff>
--- a/data/output_excels/2025-12-22_to_2025-12-28/SEBI.xlsx
+++ b/data/output_excels/2025-12-22_to_2025-12-28/SEBI.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,291 +490,46 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>January</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Ease of doing investment - Review of simplification of procedure and standardization of formats of documents for issuance of duplicate certificates</t>
+          <t>Specification of the consequential requirements with respect to Amendment of Securities and Exchange Board of India (Merchant Bankers) Regulations, 1992</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.sebi.gov.in/sebi_data/attachdocs/dec-2025/1766582923860.pdf</t>
+          <t>https://www.sebi.gov.in/sebi_data/attachdocs/jan-2026/1767358255887.pdf</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1766582923860.pdf</t>
+          <t>1767358255887.pdf</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/December/1766582923860.pdf</t>
+          <t>C:\Users\Admin\Downloads\Tejomaya_pdfs\Akshayam Data\SEBI\Circulars\2026\January\1767358255887.pdf</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>• SEBI has issued a circular to ease the process for issuing duplicate securities certificates.
-• The threshold for simplified documentation has been increased from Rs. Five Lakhs to Rs. Ten Lakhs.
-• SEBI has prescribed a standardized Affidavit-cum-Indemnity bond and rationalized documentation for securities with value over Rs. Ten Lakhs. Notarization of the affidavit is no longer required for cases involving securities up to Rs. Ten Thousand.
-• Listed companies and RTAs should process all requests strictly in accordance with the outlined procedure, and these measures are intended to facilitate investor rights and increase dematerialisation.</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>CIRCULAR
-HO/38/13/11(3)2025-MIRSD-POD/I/1102/2025 December 24, 2025
-To, All Listed Companies
-All Registrars to an Issue and Share Transfer Agents
-Madam / Sir,
-Sub: Ease of doing investment - Review of simplification of procedure and standardization of formats of documents for issuance of duplicate certificates
-1. SEBI, vide circular no. SEBI/HO/MIRSD/MIRSD_RTAMB/P/CIR/2022/70 dated
-May 25, 2022, read with Para 22 of Master Circular for Registrars to an Issue and Share Transfer Agents (‘RTAs’) dated June 23, 2025 (‘master circular’), prescribed the documentary, procedural requirements and threshold for such issuance.
-2. With the objective of further simplifying the procedure of issuance of duplicate securities and to make it more efficient and investor friendly, it was decided to review the threshold and to simplify the documentation for issuance of duplicate securities certificates.
-3. To facilitate ease of doing investment for investors, it has been decided to increase
-the threshold for simplified documentation from the current Rs. Five Lakhs to Rs. Ten Lakhs;
-4. To simplify the documentation, it has been decided to:
-4.1. prescribe a standardised Affidavit-cum-Indemnity bond;
-4.2. rationalise the documentation for securities having value of more than Rs.
-Ten Lakhs; and
-4.3. do away with notarisation of the Affidavit-cum-Indemnity bond for cases
-involving securities with value up to Rs. Ten Thousand.
-5. These measures aim at ease of investments for investors and facilitate restitution
-of investor rights in securities. As duplicate securities issued would necessarily be
-in demat mode, this will result in increased dematerialisation.
-Page 1 of 6
-6. The listed company/RTA shall process all requests for issuance of duplicate
-securities strictly in accordance with the procedure laid down here.
-7. The provisions of this circular shall come into force with immediate effect. The
-revised provisions shall also be made applicable to ongoing requests for issuance
-of duplicate securities which are under process to give benefit of the simplified
-procedure to the investors. However, if certain documents have already been
-submitted by the investor, listed companies/RTAs shall not insist on re-submission
-of such documents in the new formats.
-8. To give effect to this in the master circular Para 22.1.1 to 22.1.4 shall stand
-substituted by the following para:
-“Para 22.1.1
-If the value of securities as on the date of submission of application, along with
-complete documentation as prescribed by the Board does not exceed Rs.Ten
-Lakhs, the security holder shall submit an Affidavit-cum-Indemnity bond as per
-the format prescribed at Annexure-A, on a non-judicial stamp paper of
-appropriate value as prescribed by the Stamp Act of the state where the
-claimant resides.
-The value of the non-judicial stamp paper shall be reckoned as higher of the
-amount as prescribed for an affidavit and an indemnity individually”
-Para 22.1.2
-Further, for securities having value up to Rs. Ten Thousand, as on the date of
-submission of application, the security holder shall submit an undertaking as
-per format specified at Annexure-A on a plain paper.”
-Para 22.1.3 For securities having value more than Rs. Ten Lakhs, the claimant shall, in
-addition to the document mentioned in Para 22.1.1, submit a copy of FIR including e-FIR/Police complaint/Court injunction order/copy of plaint (where
-the suit filed has been accepted by the Court and Suit No. has been given), necessarily having details of the securities, folio number, distinctive number
-range and certificate numbers.
-Page 2 of 6
-Para 22.1.4 For securities having value more than Rs. Ten Lakhs, the listed company shall
-issue an advertisement regarding loss of securities in a widely circulated newspaper in the region where its registered office is situated, on a weekly
-basis. The timeline for processing of the service request for issuance of duplicate security certificates shall commence from the date of submission of
-complete documentation by the investor or issuance of newspaper publication by the listed company, whichever is later.
-The listed company may charge a minimal fee from the investor towards such advertisement.”
-9. This circular is issued in exercise of powers conferred under Section 11(1) of
-Chapter IV of the Securities and Exchange Board of India Act, 1992 read with
-Regulation 37 of Securities and Exchange Board of India (Registrars to an Issue
-and Share Transfer Agents) Regulations, 2025, to protect the interests of investors
-in securities and to promote the development of, and to regulate the securities
-markets.
-10. This circular is available on SEBI website at www.sebi.gov.in under the category:
-‘Legal → Circulars’.
-Yours faithfully,
-Aradhana Verma
-General Manager
-Market Intermediaries Regulation and Supervision Department
-Tel. No. 022-2644-9633
-Email id – aradhanad@sebi.gov.in
-Page 3 of 6
-Annexure-A
-Format for Affidavit-cum-Indemnity
-FORM–A
-AFFIDAVIT-CUM-INDEMNITY
-[For issuance of duplicate securities]
-Note: This affidavit is to be executed in the presence of a Public Notary (in cases where the value of securities exceeds Rs. Ten Thousand)
-[To be submitted in non-judicial stamp paper of appropriate value as prescribed by the Stamp Act of the state where the claimant resides (in cases where the value of securities exceeds Rs. Ten Thousand)]
-I/We,_______________________________________________________
-Son / daughter/spouse of ____________________________________________________ residing at ___________________________________________________________________ ___________________________________________________________________ ______________________________, having Permanent Account No (s) ______________________________do hereby solemnly affirm and state on oath as follows.
-1. That I/We, _________________________________________ (“all the shareholders ”) hold the following (number of) securities under Folio no. _____ in (name of the company) in my/ our name as single holder / joint holder:
-Compan y Name
-Folio Number
-Number and face value of securities held
-Security Certificat e No.
-Distinctive Nos.
-From
-To
-1)
-2)
-3)
-2. I/We_____________________________________________________________ ________ swear / solemnly declare that the above securities were acquired by
-Page 4 of 6
-me/us for valuable consideration out of my/our own investment/funds against allotment in Public Issue/allotment in Right Issue or acquired from the market/through inheritance in the year(s).
-3. I/We_____________________________________________________________ ________ further swear / solemnly declare that I/ we am/are applying for issue of duplicate certificate(s) to me/us on the ground that the original security(ies) certificate(s) has/have been misplaced / not found by me/us, despite a diligent search made by me/us in this behalf.
-4. I/We_____________________________________________________________ __________ further swear /solemnly declare that the said securities are not sold or pledged or deposited by way of security to any person/company.
-5. I/We_____________________________________________________________ __________________hereby further swear / solemnly declare that if, after the duplicate share certificate(s) is / are issued to us as aforesaid, the original security(ies) certificate(s) is / are at any time subsequently, found, recovered or traced by us or by anyone on our behalf, then, we unconditionally undertake not to deal with the said original share certificate(s) in any manner whatsoever (whether by physical transfer or dematerialization or as security or pledge) and further unconditionally undertake to promptly surrender the original share certificate(s) to the RTA / Company, for cancellation.
-6. I/We
-_________________________________________________________am/are making the above solemn declaration on oath with full knowledge of the fact that in the event the original security (ies) certificate(s) issued is /are found, recovered and traced by me/us and instead of surrendering the same is / are dealt with by me/us as aforesaid, the Company will be at liberty to adopt civil and / or criminal proceedings against me/us for my/our failure to promptly surrender the original security (ies) certificate(s), for cancellation and for breach of my/our solemn declaration and undertaking not to deal with the original security (ies) certificate(s) in any manner whatsoever as aforesaid at my/our entire risk as to cost and consequences.
-7. I/We hereby jointly and severely agree and undertake to indemnify and keep indemnified, saved, defended, harmless, the Company/RTA) and its successors and assigns for all time hereafter against all losses, costs, claims, actions, demands, risks, charges, expenses, damages, etc., whatsoever which you may suffer and/or incur by reason of your, at my/our request, issuing the said Duplicate Securities as herein above mentioned, to the undersigned. (Name of
-Page 5 of 6
-Signature of all deponents : X________________ ________________ ________________
-VERIFICATION
-We hereby solemnly affirm and state that what is stated herein above is true to our knowledge and nothing has been concealed therein and that we are competent to contract and entitled to rights and benefits of the above mentioned securities.
-IN WITNESS WHEREOF the said 1) Mr. /Ms. _______ (Name and signature of the witness) ____________________________ And 2) Mr. /Ms. ________________________ Name and signature of the witness ______ #, have hereunto set their respective hands and seals this day of _____________________________
-Address of First holder / Applicant :
-Signature of All holder(s) / Applicant(s) :
-_____________________________________
-___________________________________
-______________________________________Pinc ode
-_____________________________________
-FOR OFFICE USE ONLY
-Signature checked by :
-Signed before me
-at: __________________________
-on:: ___________________________
-Signed before me
-Place: __________________________
-Date : ___________________________
-X --------------------------------------------------
-Signature of Notary with Official Seal of Notary &amp; Regn. No.
-Page 6 of 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SEBI</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Circulars</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-12-24</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Ease of investments and ease of doing business measures – enhancing the ‘Facility for Basic Services Demat Account (BSDA)’</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://www.sebi.gov.in/sebi_data/attachdocs/dec-2025/1766582690382.pdf</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>1766582690382.pdf</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/December/1766582690382.pdf</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>• Starting from March 31, 2026, depository participants (DPs) can exclude Zero Coupon Zero Principal (ZCZP) bonds and delisted securities for reckoning the BSDA threshold.
-• The valuation of illiquid securities will now be at the last closing price for calculating the BSDA threshold.
-• DPs are required to reassess the BSDA eligibility every quarter and have the beneficiary owner submit consent to avail or continue to avail the facility of a regular demat account by active consent through a verifiable channel as specified by the Depositories.
-• The Depositories must make amendments to their relevant bye-laws, rules, and regulations for the implementation of these changes immediately. (SEBI has issued a circular to ease investments and doing business in the securities market by enhancing the 'Facility for Basic Services Demat Account (BSDA)' is not concrete enough to be included.)</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>CIRCULAR
-HO/38/11/11(3)2025-MIRSD-POD/I/1101/2025 December 24, 2025
-To,
-All Depositories All Depository Participants (DPs) through Depositories
-Madam / Sir,
-Subject: Ease of investments and ease of doing business measures – enhancing the ‘Facility for Basic Services Demat Account (BSDA)’
-1. SEBI, vide circular no. SEBI/HO/MIRSD/MIRSD-PoD1/P/CIR/2024/91 dated June 28, 2024 (‘the circular’), specified provisions related to enhancing the facility of BSDA to boost investor participation in securities market. SEBI received stakeholder inputs for further enhancing the facility of BSDA.
-2. Thus in order to provide ease of doing business to the depository participants (DPs)
-and ease of doing investments for the investors, it has been decided to exclude the following securities for reckoning the threshold for BSDA
-2.1. Zero Coupon Zero Principal (ZCZP) bonds
-2.2. Delisted securities
-3. The valuation of the illiquid securities shall be at last closing price for calculating
-the threshold for BSDA; and
-4. DPs shall now be required to reassess the BSDA eligibility every quarter.
-5. DPs shall require the beneficiary owner to submit consent to avail / continue to
-avail the facility of a regular demat account by active consent through a verifiable channel as specified by the Depositories.
-6. The effect of this circular shall replace paras 2.2(a), 2.2(b) and 2.3(c) of the circular,
-which stand modified as under:
-Para 2.2(a)
-The DPs shall open only BSDA for Beneficial Owners (BOs), if such demat
-accounts are eligible for BSDA as per para 2.1 above, unless such BOs specifically
-Page 1 of 3
-provide their consent through authenticated and verifiable channel to avail the
-facility of a regular demat account.
-Para 2.2(b)
-The DPs shall also reassess the eligibility of all the existing BOs with respect to
-BSDA as provided in para 2.1 above at the end of every quarter and shall convert
-all such eligible demat accounts into BSDA unless such BOs specifically provide
-their consent through authenticated and verifiable channel, as specified by
-Depositories, to continue to avail the facility of a regular demat account.
-Para 2.3(c)
-The value of holding shall be determined by the DPs on the basis of the daily
-closing price or NAV of the securities or units of mutual funds, as the case may be.
-Where such price is not available, the last traded price may be taken into account.
-For unlisted securities other than units of mutual funds, face value may be taken in
-to account. For illiquid securities, last closing price may be taken into account. The
-value of suspended securities, delisted securities and Zero Coupon Zero Principal
-bonds may not be considered for the purpose of determining eligibility of demat
-account as BSDA.
-7. The provisions of this circular shall come into force with effect from March 31, 2026
-in supersession of paras 2.2(a), 2.2(b) and 2.3(c) of the circular.
-8. The Depositories are advised to:-
-8.1. make amendments to the relevant bye-laws, rules and regulations for the
-implementation of
-the above decision
-immediately, as may be
-applicable/necessary;
-8.2. bring the provisions of this circular to the notice of their DPs and also to
-disseminate the same on their website; and
-8.3. put in place appropriate systems and procedures to give effect to the provisions
-made in this circular within a period of 75 days, and implement the provisions
-after user testing within 90 days from the date of issuance of this circular.
-9. This circular is being issued in exercise of powers conferred under section 11 (1)
-of the Securities and Exchange Board of India Act, 1992 and section 19 of the
-Page 2 of 3
-Depositories Act, 1996 to protect the interests of investors in securities and to
-promote the development of, and to regulate the securities market.
-10. This circular is available on SEBI website at www.sebi.gov.in under the category:
-‘Legal → Circulars’.
-Yours faithfully,
-Aradhana Verma
-General Manager
-Market Intermediaries Regulation and Supervision Department
-Tel. No. 022-2644-9633
-Email id – aradhanad@sebi.gov.in
-Page 3 of 3</t>
+          <t>NA</t>
         </is>
       </c>
     </row>

</xml_diff>